<commit_message>
Stuck somewhere. Not sure what's happened, but it broke. Look at later.
</commit_message>
<xml_diff>
--- a/src/com/kentcdodds/featurebuilder/resources/domoWebEndpoints.xlsx
+++ b/src/com/kentcdodds/featurebuilder/resources/domoWebEndpoints.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="domoWebEndpoints.csv" sheetId="1" r:id="rId1"/>
@@ -1069,8 +1069,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1090,19 +1098,27 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -1145,10 +1161,10 @@
     <tableColumn id="4" name="Domain" dataDxfId="2">
       <calculatedColumnFormula>IF(Table3[[#This Row],[Is Domain]],Table3[[#This Row],[Without domoweb]],LEFT(Table3[[#This Row],[Without domoweb]],FIND("/",Table3[[#This Row],[Without domoweb]])-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Is Feature" dataDxfId="0">
+    <tableColumn id="8" name="Is Feature" dataDxfId="1">
       <calculatedColumnFormula>LEN(Table3[[#This Row],[path]])-LEN(SUBSTITUTE(Table3[[#This Row],[path]],"/",""))&lt;4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Feature" dataDxfId="1">
+    <tableColumn id="5" name="Feature" dataDxfId="0">
       <calculatedColumnFormula>IF(Table3[[#This Row],[Is Domain]],Table3[[#This Row],[Domain]],RIGHT(Table3[[#This Row],[Without domoweb]],LEN(Table3[[#This Row],[Without domoweb]])-FIND("/",Table3[[#This Row],[Without domoweb]])))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1480,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H332"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>